<commit_message>
Done. Twice. For some reason. Both give basically the same output. OOS R^2 is pretty different to original paper. I don't know why. ChatGPT doesn't know why. God probably doesn't know why. I'm going to bed.
</commit_message>
<xml_diff>
--- a/data-folder/Extracted_excess_returns.xlsx
+++ b/data-folder/Extracted_excess_returns.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G641"/>
+  <dimension ref="A1:G570"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13537,1639 +13537,6 @@
         <v>-0.01920172554892209</v>
       </c>
     </row>
-    <row r="571">
-      <c r="A571" s="2" t="n">
-        <v>43466</v>
-      </c>
-      <c r="B571" t="n">
-        <v>-0.00361815549348855</v>
-      </c>
-      <c r="C571" t="n">
-        <v>-0.001158830302123097</v>
-      </c>
-      <c r="D571" t="n">
-        <v>0.003279104299574363</v>
-      </c>
-      <c r="E571" t="n">
-        <v>0.007535883895780103</v>
-      </c>
-      <c r="F571" t="n">
-        <v>0.01501787185810425</v>
-      </c>
-      <c r="G571" t="n">
-        <v>0.01372316634490593</v>
-      </c>
-    </row>
-    <row r="572">
-      <c r="A572" s="2" t="n">
-        <v>43497</v>
-      </c>
-      <c r="B572" t="n">
-        <v>-0.002730163442990392</v>
-      </c>
-      <c r="C572" t="n">
-        <v>-0.0003884569791514254</v>
-      </c>
-      <c r="D572" t="n">
-        <v>0.004965079175180572</v>
-      </c>
-      <c r="E572" t="n">
-        <v>0.009312709718082523</v>
-      </c>
-      <c r="F572" t="n">
-        <v>0.01781988581898076</v>
-      </c>
-      <c r="G572" t="n">
-        <v>0.02274964476900519</v>
-      </c>
-    </row>
-    <row r="573">
-      <c r="A573" s="2" t="n">
-        <v>43525</v>
-      </c>
-      <c r="B573" t="n">
-        <v>-0.001206663718303018</v>
-      </c>
-      <c r="C573" t="n">
-        <v>0.003550282958424175</v>
-      </c>
-      <c r="D573" t="n">
-        <v>0.01034447215486455</v>
-      </c>
-      <c r="E573" t="n">
-        <v>0.01623458907002733</v>
-      </c>
-      <c r="F573" t="n">
-        <v>0.02747472131412734</v>
-      </c>
-      <c r="G573" t="n">
-        <v>0.03702493790793634</v>
-      </c>
-    </row>
-    <row r="574">
-      <c r="A574" s="2" t="n">
-        <v>43556</v>
-      </c>
-      <c r="B574" t="n">
-        <v>0.001652537594265941</v>
-      </c>
-      <c r="C574" t="n">
-        <v>0.00948575500220427</v>
-      </c>
-      <c r="D574" t="n">
-        <v>0.01775680861273086</v>
-      </c>
-      <c r="E574" t="n">
-        <v>0.02516506161241525</v>
-      </c>
-      <c r="F574" t="n">
-        <v>0.03763437101391582</v>
-      </c>
-      <c r="G574" t="n">
-        <v>0.0473250150521449</v>
-      </c>
-    </row>
-    <row r="575">
-      <c r="A575" s="2" t="n">
-        <v>43586</v>
-      </c>
-      <c r="B575" t="n">
-        <v>0.002494204667145564</v>
-      </c>
-      <c r="C575" t="n">
-        <v>0.01402061365630342</v>
-      </c>
-      <c r="D575" t="n">
-        <v>0.02540220200486409</v>
-      </c>
-      <c r="E575" t="n">
-        <v>0.03463313953264942</v>
-      </c>
-      <c r="F575" t="n">
-        <v>0.05285189209157196</v>
-      </c>
-      <c r="G575" t="n">
-        <v>0.07265968090656724</v>
-      </c>
-    </row>
-    <row r="576">
-      <c r="A576" s="2" t="n">
-        <v>43617</v>
-      </c>
-      <c r="B576" t="n">
-        <v>0.006400419801577805</v>
-      </c>
-      <c r="C576" t="n">
-        <v>0.01855042827170435</v>
-      </c>
-      <c r="D576" t="n">
-        <v>0.03122875558995312</v>
-      </c>
-      <c r="E576" t="n">
-        <v>0.04243226680868643</v>
-      </c>
-      <c r="F576" t="n">
-        <v>0.06171338240963988</v>
-      </c>
-      <c r="G576" t="n">
-        <v>0.08339138561345455</v>
-      </c>
-    </row>
-    <row r="577">
-      <c r="A577" s="2" t="n">
-        <v>43647</v>
-      </c>
-      <c r="B577" t="n">
-        <v>0.00734961449030741</v>
-      </c>
-      <c r="C577" t="n">
-        <v>0.01943714817491468</v>
-      </c>
-      <c r="D577" t="n">
-        <v>0.03162032801929007</v>
-      </c>
-      <c r="E577" t="n">
-        <v>0.0431085869214137</v>
-      </c>
-      <c r="F577" t="n">
-        <v>0.06514135122459111</v>
-      </c>
-      <c r="G577" t="n">
-        <v>0.09252452996728515</v>
-      </c>
-    </row>
-    <row r="578">
-      <c r="A578" s="2" t="n">
-        <v>43678</v>
-      </c>
-      <c r="B578" t="n">
-        <v>0.008928788852578206</v>
-      </c>
-      <c r="C578" t="n">
-        <v>0.0243976502779591</v>
-      </c>
-      <c r="D578" t="n">
-        <v>0.04048775810980491</v>
-      </c>
-      <c r="E578" t="n">
-        <v>0.05467404664954068</v>
-      </c>
-      <c r="F578" t="n">
-        <v>0.08423860651931289</v>
-      </c>
-      <c r="G578" t="n">
-        <v>0.1291375155831178</v>
-      </c>
-    </row>
-    <row r="579">
-      <c r="A579" s="2" t="n">
-        <v>43709</v>
-      </c>
-      <c r="B579" t="n">
-        <v>0.01069854923616976</v>
-      </c>
-      <c r="C579" t="n">
-        <v>0.02592579302982608</v>
-      </c>
-      <c r="D579" t="n">
-        <v>0.04226491904957771</v>
-      </c>
-      <c r="E579" t="n">
-        <v>0.05745527685836591</v>
-      </c>
-      <c r="F579" t="n">
-        <v>0.08760002995029728</v>
-      </c>
-      <c r="G579" t="n">
-        <v>0.1315950682241088</v>
-      </c>
-    </row>
-    <row r="580">
-      <c r="A580" s="2" t="n">
-        <v>43739</v>
-      </c>
-      <c r="B580" t="n">
-        <v>0.01312075878317307</v>
-      </c>
-      <c r="C580" t="n">
-        <v>0.02838464008353938</v>
-      </c>
-      <c r="D580" t="n">
-        <v>0.04426830963584348</v>
-      </c>
-      <c r="E580" t="n">
-        <v>0.05947878117604231</v>
-      </c>
-      <c r="F580" t="n">
-        <v>0.09060221378996194</v>
-      </c>
-      <c r="G580" t="n">
-        <v>0.1388740759159746</v>
-      </c>
-    </row>
-    <row r="581">
-      <c r="A581" s="2" t="n">
-        <v>43770</v>
-      </c>
-      <c r="B581" t="n">
-        <v>0.01055663566580914</v>
-      </c>
-      <c r="C581" t="n">
-        <v>0.02259541830829126</v>
-      </c>
-      <c r="D581" t="n">
-        <v>0.03594053593464784</v>
-      </c>
-      <c r="E581" t="n">
-        <v>0.04786436443356268</v>
-      </c>
-      <c r="F581" t="n">
-        <v>0.07213380412271321</v>
-      </c>
-      <c r="G581" t="n">
-        <v>0.1150840958558855</v>
-      </c>
-    </row>
-    <row r="582">
-      <c r="A582" s="2" t="n">
-        <v>43800</v>
-      </c>
-      <c r="B582" t="n">
-        <v>0.006448267424807884</v>
-      </c>
-      <c r="C582" t="n">
-        <v>0.0147632028758328</v>
-      </c>
-      <c r="D582" t="n">
-        <v>0.02363309233811264</v>
-      </c>
-      <c r="E582" t="n">
-        <v>0.03146587561621467</v>
-      </c>
-      <c r="F582" t="n">
-        <v>0.04740581568019293</v>
-      </c>
-      <c r="G582" t="n">
-        <v>0.07377561099327137</v>
-      </c>
-    </row>
-    <row r="583">
-      <c r="A583" s="2" t="n">
-        <v>43831</v>
-      </c>
-      <c r="B583" t="n">
-        <v>0.007962729172566504</v>
-      </c>
-      <c r="C583" t="n">
-        <v>0.01983945421031807</v>
-      </c>
-      <c r="D583" t="n">
-        <v>0.03214534952861871</v>
-      </c>
-      <c r="E583" t="n">
-        <v>0.04345245915816887</v>
-      </c>
-      <c r="F583" t="n">
-        <v>0.0674513191293778</v>
-      </c>
-      <c r="G583" t="n">
-        <v>0.1045968477384557</v>
-      </c>
-    </row>
-    <row r="584">
-      <c r="A584" s="2" t="n">
-        <v>43862</v>
-      </c>
-      <c r="B584" t="n">
-        <v>0.01344064527575385</v>
-      </c>
-      <c r="C584" t="n">
-        <v>0.02990160801104435</v>
-      </c>
-      <c r="D584" t="n">
-        <v>0.0468049890197291</v>
-      </c>
-      <c r="E584" t="n">
-        <v>0.06274428834093522</v>
-      </c>
-      <c r="F584" t="n">
-        <v>0.09638939937313974</v>
-      </c>
-      <c r="G584" t="n">
-        <v>0.1423741311584278</v>
-      </c>
-    </row>
-    <row r="585">
-      <c r="A585" s="2" t="n">
-        <v>43891</v>
-      </c>
-      <c r="B585" t="n">
-        <v>0.01989626719949985</v>
-      </c>
-      <c r="C585" t="n">
-        <v>0.0373350816314017</v>
-      </c>
-      <c r="D585" t="n">
-        <v>0.0554369586554599</v>
-      </c>
-      <c r="E585" t="n">
-        <v>0.0734626831304221</v>
-      </c>
-      <c r="F585" t="n">
-        <v>0.1081278574561396</v>
-      </c>
-      <c r="G585" t="n">
-        <v>0.1543921634414548</v>
-      </c>
-    </row>
-    <row r="586">
-      <c r="A586" s="2" t="n">
-        <v>43922</v>
-      </c>
-      <c r="B586" t="n">
-        <v>0.01987466545831065</v>
-      </c>
-      <c r="C586" t="n">
-        <v>0.03875343176984759</v>
-      </c>
-      <c r="D586" t="n">
-        <v>0.05828344086717956</v>
-      </c>
-      <c r="E586" t="n">
-        <v>0.07677465770515711</v>
-      </c>
-      <c r="F586" t="n">
-        <v>0.1148258027185455</v>
-      </c>
-      <c r="G586" t="n">
-        <v>0.1684724833838844</v>
-      </c>
-    </row>
-    <row r="587">
-      <c r="A587" s="2" t="n">
-        <v>43952</v>
-      </c>
-      <c r="B587" t="n">
-        <v>0.0146613914231862</v>
-      </c>
-      <c r="C587" t="n">
-        <v>0.03057982003916971</v>
-      </c>
-      <c r="D587" t="n">
-        <v>0.04749672333031989</v>
-      </c>
-      <c r="E587" t="n">
-        <v>0.06353478358762418</v>
-      </c>
-      <c r="F587" t="n">
-        <v>0.09299210812807723</v>
-      </c>
-      <c r="G587" t="n">
-        <v>0.133629802990397</v>
-      </c>
-    </row>
-    <row r="588">
-      <c r="A588" s="2" t="n">
-        <v>43983</v>
-      </c>
-      <c r="B588" t="n">
-        <v>0.01418202271681154</v>
-      </c>
-      <c r="C588" t="n">
-        <v>0.02901689304843611</v>
-      </c>
-      <c r="D588" t="n">
-        <v>0.04459284402837574</v>
-      </c>
-      <c r="E588" t="n">
-        <v>0.06030564958506929</v>
-      </c>
-      <c r="F588" t="n">
-        <v>0.08729398675907851</v>
-      </c>
-      <c r="G588" t="n">
-        <v>0.1243227125826994</v>
-      </c>
-    </row>
-    <row r="589">
-      <c r="A589" s="2" t="n">
-        <v>44013</v>
-      </c>
-      <c r="B589" t="n">
-        <v>0.01596505337763098</v>
-      </c>
-      <c r="C589" t="n">
-        <v>0.03210177215597325</v>
-      </c>
-      <c r="D589" t="n">
-        <v>0.04890754070366386</v>
-      </c>
-      <c r="E589" t="n">
-        <v>0.06439898457075138</v>
-      </c>
-      <c r="F589" t="n">
-        <v>0.09399679728132629</v>
-      </c>
-      <c r="G589" t="n">
-        <v>0.1355168453924639</v>
-      </c>
-    </row>
-    <row r="590">
-      <c r="A590" s="2" t="n">
-        <v>44044</v>
-      </c>
-      <c r="B590" t="n">
-        <v>0.01145298989463135</v>
-      </c>
-      <c r="C590" t="n">
-        <v>0.02218191186502627</v>
-      </c>
-      <c r="D590" t="n">
-        <v>0.03373668605888183</v>
-      </c>
-      <c r="E590" t="n">
-        <v>0.04362976105371989</v>
-      </c>
-      <c r="F590" t="n">
-        <v>0.05895534370012459</v>
-      </c>
-      <c r="G590" t="n">
-        <v>0.07340303926680168</v>
-      </c>
-    </row>
-    <row r="591">
-      <c r="A591" s="2" t="n">
-        <v>44075</v>
-      </c>
-      <c r="B591" t="n">
-        <v>0.01360463656048575</v>
-      </c>
-      <c r="C591" t="n">
-        <v>0.0262920914600755</v>
-      </c>
-      <c r="D591" t="n">
-        <v>0.03909517250425927</v>
-      </c>
-      <c r="E591" t="n">
-        <v>0.05093583880171372</v>
-      </c>
-      <c r="F591" t="n">
-        <v>0.07075221607061934</v>
-      </c>
-      <c r="G591" t="n">
-        <v>0.09258464474184205</v>
-      </c>
-    </row>
-    <row r="592">
-      <c r="A592" s="2" t="n">
-        <v>44105</v>
-      </c>
-      <c r="B592" t="n">
-        <v>0.01346523224810711</v>
-      </c>
-      <c r="C592" t="n">
-        <v>0.02600934005040033</v>
-      </c>
-      <c r="D592" t="n">
-        <v>0.03831689303462068</v>
-      </c>
-      <c r="E592" t="n">
-        <v>0.04859388002876009</v>
-      </c>
-      <c r="F592" t="n">
-        <v>0.06309371768465008</v>
-      </c>
-      <c r="G592" t="n">
-        <v>0.07955997931236647</v>
-      </c>
-    </row>
-    <row r="593">
-      <c r="A593" s="2" t="n">
-        <v>44136</v>
-      </c>
-      <c r="B593" t="n">
-        <v>0.01487583642620378</v>
-      </c>
-      <c r="C593" t="n">
-        <v>0.02824436155063763</v>
-      </c>
-      <c r="D593" t="n">
-        <v>0.04211637644056473</v>
-      </c>
-      <c r="E593" t="n">
-        <v>0.05387496460241895</v>
-      </c>
-      <c r="F593" t="n">
-        <v>0.07265450320041729</v>
-      </c>
-      <c r="G593" t="n">
-        <v>0.09129779979391082</v>
-      </c>
-    </row>
-    <row r="594">
-      <c r="A594" s="2" t="n">
-        <v>44166</v>
-      </c>
-      <c r="B594" t="n">
-        <v>0.01451952313494081</v>
-      </c>
-      <c r="C594" t="n">
-        <v>0.02950651166279436</v>
-      </c>
-      <c r="D594" t="n">
-        <v>0.04498535969005632</v>
-      </c>
-      <c r="E594" t="n">
-        <v>0.05772090818992801</v>
-      </c>
-      <c r="F594" t="n">
-        <v>0.07948720934565034</v>
-      </c>
-      <c r="G594" t="n">
-        <v>0.1004128193941855</v>
-      </c>
-    </row>
-    <row r="595">
-      <c r="A595" s="2" t="n">
-        <v>44197</v>
-      </c>
-      <c r="B595" t="n">
-        <v>0.01072464539033614</v>
-      </c>
-      <c r="C595" t="n">
-        <v>0.02118642345234453</v>
-      </c>
-      <c r="D595" t="n">
-        <v>0.03131263879346636</v>
-      </c>
-      <c r="E595" t="n">
-        <v>0.03869390087778386</v>
-      </c>
-      <c r="F595" t="n">
-        <v>0.04599093581636202</v>
-      </c>
-      <c r="G595" t="n">
-        <v>0.04565792689781992</v>
-      </c>
-    </row>
-    <row r="596">
-      <c r="A596" s="2" t="n">
-        <v>44228</v>
-      </c>
-      <c r="B596" t="n">
-        <v>0.006678049019212838</v>
-      </c>
-      <c r="C596" t="n">
-        <v>0.01288801375213907</v>
-      </c>
-      <c r="D596" t="n">
-        <v>0.01662323259980147</v>
-      </c>
-      <c r="E596" t="n">
-        <v>0.01461726716729373</v>
-      </c>
-      <c r="F596" t="n">
-        <v>0.003407341291963129</v>
-      </c>
-      <c r="G596" t="n">
-        <v>-0.01755174561148948</v>
-      </c>
-    </row>
-    <row r="597">
-      <c r="A597" s="2" t="n">
-        <v>44256</v>
-      </c>
-      <c r="B597" t="n">
-        <v>0.002550675772559071</v>
-      </c>
-      <c r="C597" t="n">
-        <v>0.003731219204648599</v>
-      </c>
-      <c r="D597" t="n">
-        <v>0.0005271364184803893</v>
-      </c>
-      <c r="E597" t="n">
-        <v>-0.009195102335765939</v>
-      </c>
-      <c r="F597" t="n">
-        <v>-0.03853808166980331</v>
-      </c>
-      <c r="G597" t="n">
-        <v>-0.08499127164041669</v>
-      </c>
-    </row>
-    <row r="598">
-      <c r="A598" s="2" t="n">
-        <v>44287</v>
-      </c>
-      <c r="B598" t="n">
-        <v>0.001761846315069069</v>
-      </c>
-      <c r="C598" t="n">
-        <v>0.002257037761306121</v>
-      </c>
-      <c r="D598" t="n">
-        <v>0.000296269209097322</v>
-      </c>
-      <c r="E598" t="n">
-        <v>-0.008140648807590446</v>
-      </c>
-      <c r="F598" t="n">
-        <v>-0.03314343515743521</v>
-      </c>
-      <c r="G598" t="n">
-        <v>-0.08099110922927963</v>
-      </c>
-    </row>
-    <row r="599">
-      <c r="A599" s="2" t="n">
-        <v>44317</v>
-      </c>
-      <c r="B599" t="n">
-        <v>0.0008939432577551856</v>
-      </c>
-      <c r="C599" t="n">
-        <v>0.0009318424416118912</v>
-      </c>
-      <c r="D599" t="n">
-        <v>-0.001817308021765678</v>
-      </c>
-      <c r="E599" t="n">
-        <v>-0.009387716688977702</v>
-      </c>
-      <c r="F599" t="n">
-        <v>-0.03295773918229988</v>
-      </c>
-      <c r="G599" t="n">
-        <v>-0.07847484703634246</v>
-      </c>
-    </row>
-    <row r="600">
-      <c r="A600" s="2" t="n">
-        <v>44348</v>
-      </c>
-      <c r="B600" t="n">
-        <v>0.0001713458986355031</v>
-      </c>
-      <c r="C600" t="n">
-        <v>-0.002030972392199407</v>
-      </c>
-      <c r="D600" t="n">
-        <v>-0.00792053610088049</v>
-      </c>
-      <c r="E600" t="n">
-        <v>-0.01589087292118995</v>
-      </c>
-      <c r="F600" t="n">
-        <v>-0.03454671826763843</v>
-      </c>
-      <c r="G600" t="n">
-        <v>-0.06729818202976302</v>
-      </c>
-    </row>
-    <row r="601">
-      <c r="A601" s="2" t="n">
-        <v>44378</v>
-      </c>
-      <c r="B601" t="n">
-        <v>8.6142595205442e-05</v>
-      </c>
-      <c r="C601" t="n">
-        <v>-0.001701749702140241</v>
-      </c>
-      <c r="D601" t="n">
-        <v>-0.005627788464915271</v>
-      </c>
-      <c r="E601" t="n">
-        <v>-0.0128018524390765</v>
-      </c>
-      <c r="F601" t="n">
-        <v>-0.02750909440756312</v>
-      </c>
-      <c r="G601" t="n">
-        <v>-0.05608427266244786</v>
-      </c>
-    </row>
-    <row r="602">
-      <c r="A602" s="2" t="n">
-        <v>44409</v>
-      </c>
-      <c r="B602" t="n">
-        <v>0.0002672954631123587</v>
-      </c>
-      <c r="C602" t="n">
-        <v>-0.00159110834380518</v>
-      </c>
-      <c r="D602" t="n">
-        <v>-0.006025193824046176</v>
-      </c>
-      <c r="E602" t="n">
-        <v>-0.01342718894643885</v>
-      </c>
-      <c r="F602" t="n">
-        <v>-0.02552752141818927</v>
-      </c>
-      <c r="G602" t="n">
-        <v>-0.04540700122867745</v>
-      </c>
-    </row>
-    <row r="603">
-      <c r="A603" s="2" t="n">
-        <v>44440</v>
-      </c>
-      <c r="B603" t="n">
-        <v>0.0001401379966488787</v>
-      </c>
-      <c r="C603" t="n">
-        <v>-0.002548218050103343</v>
-      </c>
-      <c r="D603" t="n">
-        <v>-0.009170682450463449</v>
-      </c>
-      <c r="E603" t="n">
-        <v>-0.01949245780804934</v>
-      </c>
-      <c r="F603" t="n">
-        <v>-0.03894822229506483</v>
-      </c>
-      <c r="G603" t="n">
-        <v>-0.06494846329065351</v>
-      </c>
-    </row>
-    <row r="604">
-      <c r="A604" s="2" t="n">
-        <v>44470</v>
-      </c>
-      <c r="B604" t="n">
-        <v>-0.0004410771207716446</v>
-      </c>
-      <c r="C604" t="n">
-        <v>-0.006313180079417387</v>
-      </c>
-      <c r="D604" t="n">
-        <v>-0.01403931539146129</v>
-      </c>
-      <c r="E604" t="n">
-        <v>-0.02395629992568006</v>
-      </c>
-      <c r="F604" t="n">
-        <v>-0.03908057824738664</v>
-      </c>
-      <c r="G604" t="n">
-        <v>-0.05143834683349929</v>
-      </c>
-    </row>
-    <row r="605">
-      <c r="A605" s="2" t="n">
-        <v>44501</v>
-      </c>
-      <c r="B605" t="n">
-        <v>-0.001113153554406532</v>
-      </c>
-      <c r="C605" t="n">
-        <v>-0.00777109727192353</v>
-      </c>
-      <c r="D605" t="n">
-        <v>-0.01680412917701101</v>
-      </c>
-      <c r="E605" t="n">
-        <v>-0.02625686914374316</v>
-      </c>
-      <c r="F605" t="n">
-        <v>-0.03723410367977301</v>
-      </c>
-      <c r="G605" t="n">
-        <v>-0.04532983285871296</v>
-      </c>
-    </row>
-    <row r="606">
-      <c r="A606" s="2" t="n">
-        <v>44531</v>
-      </c>
-      <c r="B606" t="n">
-        <v>-0.003191212164630148</v>
-      </c>
-      <c r="C606" t="n">
-        <v>-0.01170651889403094</v>
-      </c>
-      <c r="D606" t="n">
-        <v>-0.02094714324134661</v>
-      </c>
-      <c r="E606" t="n">
-        <v>-0.03044953799888047</v>
-      </c>
-      <c r="F606" t="n">
-        <v>-0.03910439361969932</v>
-      </c>
-      <c r="G606" t="n">
-        <v>-0.04168057164117673</v>
-      </c>
-    </row>
-    <row r="607">
-      <c r="A607" s="2" t="n">
-        <v>44562</v>
-      </c>
-      <c r="B607" t="n">
-        <v>-0.007456649362776337</v>
-      </c>
-      <c r="C607" t="n">
-        <v>-0.02034493727805287</v>
-      </c>
-      <c r="D607" t="n">
-        <v>-0.03220954808429215</v>
-      </c>
-      <c r="E607" t="n">
-        <v>-0.04231788978796427</v>
-      </c>
-      <c r="F607" t="n">
-        <v>-0.05151106981891433</v>
-      </c>
-      <c r="G607" t="n">
-        <v>-0.05240557751491073</v>
-      </c>
-    </row>
-    <row r="608">
-      <c r="A608" s="2" t="n">
-        <v>44593</v>
-      </c>
-      <c r="B608" t="n">
-        <v>-0.009772810010032147</v>
-      </c>
-      <c r="C608" t="n">
-        <v>-0.02289750489800227</v>
-      </c>
-      <c r="D608" t="n">
-        <v>-0.03052307338377866</v>
-      </c>
-      <c r="E608" t="n">
-        <v>-0.0339375502512893</v>
-      </c>
-      <c r="F608" t="n">
-        <v>-0.0307243168583406</v>
-      </c>
-      <c r="G608" t="n">
-        <v>-0.0219675704559103</v>
-      </c>
-    </row>
-    <row r="609">
-      <c r="A609" s="2" t="n">
-        <v>44621</v>
-      </c>
-      <c r="B609" t="n">
-        <v>-0.01631262753479864</v>
-      </c>
-      <c r="C609" t="n">
-        <v>-0.03908081780448446</v>
-      </c>
-      <c r="D609" t="n">
-        <v>-0.05184466327178154</v>
-      </c>
-      <c r="E609" t="n">
-        <v>-0.05600093061276228</v>
-      </c>
-      <c r="F609" t="n">
-        <v>-0.05054594695418144</v>
-      </c>
-      <c r="G609" t="n">
-        <v>-0.03517321213732585</v>
-      </c>
-    </row>
-    <row r="610">
-      <c r="A610" s="2" t="n">
-        <v>44652</v>
-      </c>
-      <c r="B610" t="n">
-        <v>-0.02044454086527435</v>
-      </c>
-      <c r="C610" t="n">
-        <v>-0.04708717486019422</v>
-      </c>
-      <c r="D610" t="n">
-        <v>-0.06584505622927672</v>
-      </c>
-      <c r="E610" t="n">
-        <v>-0.07816100883563067</v>
-      </c>
-      <c r="F610" t="n">
-        <v>-0.0895408573872947</v>
-      </c>
-      <c r="G610" t="n">
-        <v>-0.09874641528222421</v>
-      </c>
-    </row>
-    <row r="611">
-      <c r="A611" s="2" t="n">
-        <v>44682</v>
-      </c>
-      <c r="B611" t="n">
-        <v>-0.02048850559104273</v>
-      </c>
-      <c r="C611" t="n">
-        <v>-0.04419019393660339</v>
-      </c>
-      <c r="D611" t="n">
-        <v>-0.06223628401170366</v>
-      </c>
-      <c r="E611" t="n">
-        <v>-0.07392524571997225</v>
-      </c>
-      <c r="F611" t="n">
-        <v>-0.08612284968829401</v>
-      </c>
-      <c r="G611" t="n">
-        <v>-0.09385918278515724</v>
-      </c>
-    </row>
-    <row r="612">
-      <c r="A612" s="2" t="n">
-        <v>44713</v>
-      </c>
-      <c r="B612" t="n">
-        <v>-0.0268029874156631</v>
-      </c>
-      <c r="C612" t="n">
-        <v>-0.04895003099027216</v>
-      </c>
-      <c r="D612" t="n">
-        <v>-0.06627682247565413</v>
-      </c>
-      <c r="E612" t="n">
-        <v>-0.08032513622882555</v>
-      </c>
-      <c r="F612" t="n">
-        <v>-0.1008617083061189</v>
-      </c>
-      <c r="G612" t="n">
-        <v>-0.1225551298770484</v>
-      </c>
-    </row>
-    <row r="613">
-      <c r="A613" s="2" t="n">
-        <v>44743</v>
-      </c>
-      <c r="B613" t="n">
-        <v>-0.02881660280791381</v>
-      </c>
-      <c r="C613" t="n">
-        <v>-0.05018926104815184</v>
-      </c>
-      <c r="D613" t="n">
-        <v>-0.06498470802189561</v>
-      </c>
-      <c r="E613" t="n">
-        <v>-0.07594842179740166</v>
-      </c>
-      <c r="F613" t="n">
-        <v>-0.09448318714485598</v>
-      </c>
-      <c r="G613" t="n">
-        <v>-0.1133168318251812</v>
-      </c>
-    </row>
-    <row r="614">
-      <c r="A614" s="2" t="n">
-        <v>44774</v>
-      </c>
-      <c r="B614" t="n">
-        <v>-0.03343876262578716</v>
-      </c>
-      <c r="C614" t="n">
-        <v>-0.06083731541566452</v>
-      </c>
-      <c r="D614" t="n">
-        <v>-0.08348731876533191</v>
-      </c>
-      <c r="E614" t="n">
-        <v>-0.1012704161447444</v>
-      </c>
-      <c r="F614" t="n">
-        <v>-0.1283972387646043</v>
-      </c>
-      <c r="G614" t="n">
-        <v>-0.1568003866224531</v>
-      </c>
-    </row>
-    <row r="615">
-      <c r="A615" s="2" t="n">
-        <v>44805</v>
-      </c>
-      <c r="B615" t="n">
-        <v>-0.04098170076187452</v>
-      </c>
-      <c r="C615" t="n">
-        <v>-0.07489737042951847</v>
-      </c>
-      <c r="D615" t="n">
-        <v>-0.1008319313307354</v>
-      </c>
-      <c r="E615" t="n">
-        <v>-0.1216463897193343</v>
-      </c>
-      <c r="F615" t="n">
-        <v>-0.1561455959946701</v>
-      </c>
-      <c r="G615" t="n">
-        <v>-0.196647502779933</v>
-      </c>
-    </row>
-    <row r="616">
-      <c r="A616" s="2" t="n">
-        <v>44835</v>
-      </c>
-      <c r="B616" t="n">
-        <v>-0.0411459756741926</v>
-      </c>
-      <c r="C616" t="n">
-        <v>-0.07185435447136068</v>
-      </c>
-      <c r="D616" t="n">
-        <v>-0.09608502481817913</v>
-      </c>
-      <c r="E616" t="n">
-        <v>-0.1172729330176823</v>
-      </c>
-      <c r="F616" t="n">
-        <v>-0.1545278956324166</v>
-      </c>
-      <c r="G616" t="n">
-        <v>-0.209389051845476</v>
-      </c>
-    </row>
-    <row r="617">
-      <c r="A617" s="2" t="n">
-        <v>44866</v>
-      </c>
-      <c r="B617" t="n">
-        <v>-0.04108846484132705</v>
-      </c>
-      <c r="C617" t="n">
-        <v>-0.0656974317190957</v>
-      </c>
-      <c r="D617" t="n">
-        <v>-0.08252530408824123</v>
-      </c>
-      <c r="E617" t="n">
-        <v>-0.1007919895619748</v>
-      </c>
-      <c r="F617" t="n">
-        <v>-0.1317090744251287</v>
-      </c>
-      <c r="G617" t="n">
-        <v>-0.1828740047467299</v>
-      </c>
-    </row>
-    <row r="618">
-      <c r="A618" s="2" t="n">
-        <v>44896</v>
-      </c>
-      <c r="B618" t="n">
-        <v>-0.03956203455341395</v>
-      </c>
-      <c r="C618" t="n">
-        <v>-0.06596394293003272</v>
-      </c>
-      <c r="D618" t="n">
-        <v>-0.08549134830885798</v>
-      </c>
-      <c r="E618" t="n">
-        <v>-0.1054359713158983</v>
-      </c>
-      <c r="F618" t="n">
-        <v>-0.1450431420692342</v>
-      </c>
-      <c r="G618" t="n">
-        <v>-0.2009797252700283</v>
-      </c>
-    </row>
-    <row r="619">
-      <c r="A619" s="2" t="n">
-        <v>44927</v>
-      </c>
-      <c r="B619" t="n">
-        <v>-0.03464585697265345</v>
-      </c>
-      <c r="C619" t="n">
-        <v>-0.05254317864228734</v>
-      </c>
-      <c r="D619" t="n">
-        <v>-0.0640562430021336</v>
-      </c>
-      <c r="E619" t="n">
-        <v>-0.07692836742800971</v>
-      </c>
-      <c r="F619" t="n">
-        <v>-0.1027309634630097</v>
-      </c>
-      <c r="G619" t="n">
-        <v>-0.1419188675362515</v>
-      </c>
-    </row>
-    <row r="620">
-      <c r="A620" s="2" t="n">
-        <v>44958</v>
-      </c>
-      <c r="B620" t="n">
-        <v>-0.03590343183453415</v>
-      </c>
-      <c r="C620" t="n">
-        <v>-0.06043331634666708</v>
-      </c>
-      <c r="D620" t="n">
-        <v>-0.07849654130805839</v>
-      </c>
-      <c r="E620" t="n">
-        <v>-0.09745285982026419</v>
-      </c>
-      <c r="F620" t="n">
-        <v>-0.1324164097230508</v>
-      </c>
-      <c r="G620" t="n">
-        <v>-0.1789144181727607</v>
-      </c>
-    </row>
-    <row r="621">
-      <c r="A621" s="2" t="n">
-        <v>44986</v>
-      </c>
-      <c r="B621" t="n">
-        <v>-0.01853204360234798</v>
-      </c>
-      <c r="C621" t="n">
-        <v>-0.02433894326840057</v>
-      </c>
-      <c r="D621" t="n">
-        <v>-0.03130399580592746</v>
-      </c>
-      <c r="E621" t="n">
-        <v>-0.04191877257506541</v>
-      </c>
-      <c r="F621" t="n">
-        <v>-0.06335185595995957</v>
-      </c>
-      <c r="G621" t="n">
-        <v>-0.09650967468250055</v>
-      </c>
-    </row>
-    <row r="622">
-      <c r="A622" s="2" t="n">
-        <v>45017</v>
-      </c>
-      <c r="B622" t="n">
-        <v>-0.0167347265097415</v>
-      </c>
-      <c r="C622" t="n">
-        <v>-0.01621941331598327</v>
-      </c>
-      <c r="D622" t="n">
-        <v>-0.01519811396665351</v>
-      </c>
-      <c r="E622" t="n">
-        <v>-0.01679670710813056</v>
-      </c>
-      <c r="F622" t="n">
-        <v>-0.02352049110324586</v>
-      </c>
-      <c r="G622" t="n">
-        <v>-0.03567484992596923</v>
-      </c>
-    </row>
-    <row r="623">
-      <c r="A623" s="2" t="n">
-        <v>45047</v>
-      </c>
-      <c r="B623" t="n">
-        <v>-0.02462867594545294</v>
-      </c>
-      <c r="C623" t="n">
-        <v>-0.02895081526430964</v>
-      </c>
-      <c r="D623" t="n">
-        <v>-0.03111454928742793</v>
-      </c>
-      <c r="E623" t="n">
-        <v>-0.03570804586083023</v>
-      </c>
-      <c r="F623" t="n">
-        <v>-0.04623966502007146</v>
-      </c>
-      <c r="G623" t="n">
-        <v>-0.06532589254178056</v>
-      </c>
-    </row>
-    <row r="624">
-      <c r="A624" s="2" t="n">
-        <v>45078</v>
-      </c>
-      <c r="B624" t="n">
-        <v>-0.02633366131935159</v>
-      </c>
-      <c r="C624" t="n">
-        <v>-0.03827943497597094</v>
-      </c>
-      <c r="D624" t="n">
-        <v>-0.04350569295332199</v>
-      </c>
-      <c r="E624" t="n">
-        <v>-0.04894404206615589</v>
-      </c>
-      <c r="F624" t="n">
-        <v>-0.05964590094415224</v>
-      </c>
-      <c r="G624" t="n">
-        <v>-0.07465934684476601</v>
-      </c>
-    </row>
-    <row r="625">
-      <c r="A625" s="2" t="n">
-        <v>45108</v>
-      </c>
-      <c r="B625" t="n">
-        <v>-0.02853672184836465</v>
-      </c>
-      <c r="C625" t="n">
-        <v>-0.04520544802078461</v>
-      </c>
-      <c r="D625" t="n">
-        <v>-0.05741503998419457</v>
-      </c>
-      <c r="E625" t="n">
-        <v>-0.06803601979724323</v>
-      </c>
-      <c r="F625" t="n">
-        <v>-0.09140340775571669</v>
-      </c>
-      <c r="G625" t="n">
-        <v>-0.1228081686773081</v>
-      </c>
-    </row>
-    <row r="626">
-      <c r="A626" s="2" t="n">
-        <v>45139</v>
-      </c>
-      <c r="B626" t="n">
-        <v>-0.0215115141637721</v>
-      </c>
-      <c r="C626" t="n">
-        <v>-0.02875497778752219</v>
-      </c>
-      <c r="D626" t="n">
-        <v>-0.03412751853640649</v>
-      </c>
-      <c r="E626" t="n">
-        <v>-0.04196620530983743</v>
-      </c>
-      <c r="F626" t="n">
-        <v>-0.05935030460360876</v>
-      </c>
-      <c r="G626" t="n">
-        <v>-0.08759502321917145</v>
-      </c>
-    </row>
-    <row r="627">
-      <c r="A627" s="2" t="n">
-        <v>45170</v>
-      </c>
-      <c r="B627" t="n">
-        <v>-0.01354479181285921</v>
-      </c>
-      <c r="C627" t="n">
-        <v>-0.01738168408730771</v>
-      </c>
-      <c r="D627" t="n">
-        <v>-0.02069908641158548</v>
-      </c>
-      <c r="E627" t="n">
-        <v>-0.02652847006601551</v>
-      </c>
-      <c r="F627" t="n">
-        <v>-0.04396698466042474</v>
-      </c>
-      <c r="G627" t="n">
-        <v>-0.07449922636414878</v>
-      </c>
-    </row>
-    <row r="628">
-      <c r="A628" s="2" t="n">
-        <v>45200</v>
-      </c>
-      <c r="B628" t="n">
-        <v>-0.0136076542877562</v>
-      </c>
-      <c r="C628" t="n">
-        <v>-0.01816660597279239</v>
-      </c>
-      <c r="D628" t="n">
-        <v>-0.0230362773577911</v>
-      </c>
-      <c r="E628" t="n">
-        <v>-0.03196309015220428</v>
-      </c>
-      <c r="F628" t="n">
-        <v>-0.05568226989267994</v>
-      </c>
-      <c r="G628" t="n">
-        <v>-0.08875827051840363</v>
-      </c>
-    </row>
-    <row r="629">
-      <c r="A629" s="2" t="n">
-        <v>45231</v>
-      </c>
-      <c r="B629" t="n">
-        <v>-0.01524732180914497</v>
-      </c>
-      <c r="C629" t="n">
-        <v>-0.0221838850352971</v>
-      </c>
-      <c r="D629" t="n">
-        <v>-0.0267019116919385</v>
-      </c>
-      <c r="E629" t="n">
-        <v>-0.0342469249550825</v>
-      </c>
-      <c r="F629" t="n">
-        <v>-0.05421025028842602</v>
-      </c>
-      <c r="G629" t="n">
-        <v>-0.08116624181066484</v>
-      </c>
-    </row>
-    <row r="630">
-      <c r="A630" s="2" t="n">
-        <v>45261</v>
-      </c>
-      <c r="B630" t="n">
-        <v>-0.0087987899633786</v>
-      </c>
-      <c r="C630" t="n">
-        <v>-0.008164633555312245</v>
-      </c>
-      <c r="D630" t="n">
-        <v>-0.005970485917000404</v>
-      </c>
-      <c r="E630" t="n">
-        <v>-0.004693400334942227</v>
-      </c>
-      <c r="F630" t="n">
-        <v>-0.006699058538669977</v>
-      </c>
-      <c r="G630" t="n">
-        <v>-0.01487714179122543</v>
-      </c>
-    </row>
-    <row r="631">
-      <c r="A631" s="2" t="n">
-        <v>45292</v>
-      </c>
-      <c r="B631" t="n">
-        <v>-0.01324107085246537</v>
-      </c>
-      <c r="C631" t="n">
-        <v>-0.0174213201953813</v>
-      </c>
-      <c r="D631" t="n">
-        <v>-0.02012422632912499</v>
-      </c>
-      <c r="E631" t="n">
-        <v>-0.02357554406494518</v>
-      </c>
-      <c r="F631" t="n">
-        <v>-0.03472533780746935</v>
-      </c>
-      <c r="G631" t="n">
-        <v>-0.05435280803973049</v>
-      </c>
-    </row>
-    <row r="632">
-      <c r="A632" s="2" t="n">
-        <v>45323</v>
-      </c>
-      <c r="B632" t="n">
-        <v>-0.008293507872484444</v>
-      </c>
-      <c r="C632" t="n">
-        <v>-0.01163634905225873</v>
-      </c>
-      <c r="D632" t="n">
-        <v>-0.01353524272232762</v>
-      </c>
-      <c r="E632" t="n">
-        <v>-0.01707923257278662</v>
-      </c>
-      <c r="F632" t="n">
-        <v>-0.0279497147564812</v>
-      </c>
-      <c r="G632" t="n">
-        <v>-0.04792146098953246</v>
-      </c>
-    </row>
-    <row r="633">
-      <c r="A633" s="2" t="n">
-        <v>45352</v>
-      </c>
-      <c r="B633" t="n">
-        <v>-0.0180942107433297</v>
-      </c>
-      <c r="C633" t="n">
-        <v>-0.02744554403103774</v>
-      </c>
-      <c r="D633" t="n">
-        <v>-0.0329552031118745</v>
-      </c>
-      <c r="E633" t="n">
-        <v>-0.03987679046801737</v>
-      </c>
-      <c r="F633" t="n">
-        <v>-0.05499616632150203</v>
-      </c>
-      <c r="G633" t="n">
-        <v>-0.08021249004655095</v>
-      </c>
-    </row>
-    <row r="634">
-      <c r="A634" s="2" t="n">
-        <v>45383</v>
-      </c>
-      <c r="B634" t="n">
-        <v>-0.02262457823956755</v>
-      </c>
-      <c r="C634" t="n">
-        <v>-0.0398392683776878</v>
-      </c>
-      <c r="D634" t="n">
-        <v>-0.05307029272574714</v>
-      </c>
-      <c r="E634" t="n">
-        <v>-0.06587866555660368</v>
-      </c>
-      <c r="F634" t="n">
-        <v>-0.09146210618038805</v>
-      </c>
-      <c r="G634" t="n">
-        <v>-0.129159643659754</v>
-      </c>
-    </row>
-    <row r="635">
-      <c r="A635" s="2" t="n">
-        <v>45413</v>
-      </c>
-      <c r="B635" t="n">
-        <v>-0.0181557092203968</v>
-      </c>
-      <c r="C635" t="n">
-        <v>-0.03058073172623881</v>
-      </c>
-      <c r="D635" t="n">
-        <v>-0.03826824419661016</v>
-      </c>
-      <c r="E635" t="n">
-        <v>-0.04690234965381738</v>
-      </c>
-      <c r="F635" t="n">
-        <v>-0.06641101722345716</v>
-      </c>
-      <c r="G635" t="n">
-        <v>-0.0947246742763469</v>
-      </c>
-    </row>
-    <row r="636">
-      <c r="A636" s="2" t="n">
-        <v>45444</v>
-      </c>
-      <c r="B636" t="n">
-        <v>-0.01019470422821661</v>
-      </c>
-      <c r="C636" t="n">
-        <v>-0.01673883802686676</v>
-      </c>
-      <c r="D636" t="n">
-        <v>-0.02075805422931647</v>
-      </c>
-      <c r="E636" t="n">
-        <v>-0.02626052785594084</v>
-      </c>
-      <c r="F636" t="n">
-        <v>-0.04298329071492087</v>
-      </c>
-      <c r="G636" t="n">
-        <v>-0.07087230662363793</v>
-      </c>
-    </row>
-    <row r="637">
-      <c r="A637" s="2" t="n">
-        <v>45474</v>
-      </c>
-      <c r="B637" t="n">
-        <v>-0.006227873738288592</v>
-      </c>
-      <c r="C637" t="n">
-        <v>-0.006476350531057294</v>
-      </c>
-      <c r="D637" t="n">
-        <v>-0.005355958578291846</v>
-      </c>
-      <c r="E637" t="n">
-        <v>-0.004682984367563862</v>
-      </c>
-      <c r="F637" t="n">
-        <v>-0.009779206415336465</v>
-      </c>
-      <c r="G637" t="n">
-        <v>-0.02542744244505853</v>
-      </c>
-    </row>
-    <row r="638">
-      <c r="A638" s="2" t="n">
-        <v>45505</v>
-      </c>
-      <c r="B638" t="n">
-        <v>-0.002846139790129223</v>
-      </c>
-      <c r="C638" t="n">
-        <v>0.001217665515456351</v>
-      </c>
-      <c r="D638" t="n">
-        <v>0.005233091771755266</v>
-      </c>
-      <c r="E638" t="n">
-        <v>0.007888735923694407</v>
-      </c>
-      <c r="F638" t="n">
-        <v>0.008410481523847685</v>
-      </c>
-      <c r="G638" t="n">
-        <v>0.002385022565669498</v>
-      </c>
-    </row>
-    <row r="639">
-      <c r="A639" s="2" t="n">
-        <v>45536</v>
-      </c>
-      <c r="B639" t="n">
-        <v>0.004281684336514199</v>
-      </c>
-      <c r="C639" t="n">
-        <v>0.01375312768521436</v>
-      </c>
-      <c r="D639" t="n">
-        <v>0.02302089491603874</v>
-      </c>
-      <c r="E639" t="n">
-        <v>0.03158072408272299</v>
-      </c>
-      <c r="F639" t="n">
-        <v>0.04575865403739367</v>
-      </c>
-      <c r="G639" t="n">
-        <v>0.05864385911026938</v>
-      </c>
-    </row>
-    <row r="640">
-      <c r="A640" s="2" t="n">
-        <v>45566</v>
-      </c>
-      <c r="B640" t="n">
-        <v>0.001109669057516277</v>
-      </c>
-      <c r="C640" t="n">
-        <v>0.006596103552900204</v>
-      </c>
-      <c r="D640" t="n">
-        <v>0.01347114189119106</v>
-      </c>
-      <c r="E640" t="n">
-        <v>0.02049039563623464</v>
-      </c>
-      <c r="F640" t="n">
-        <v>0.03396332933285479</v>
-      </c>
-      <c r="G640" t="n">
-        <v>0.05057151521344005</v>
-      </c>
-    </row>
-    <row r="641">
-      <c r="A641" s="2" t="n">
-        <v>45597</v>
-      </c>
-      <c r="B641" t="n">
-        <v>-0.004643055050685185</v>
-      </c>
-      <c r="C641" t="n">
-        <v>-0.005430466515941507</v>
-      </c>
-      <c r="D641" t="n">
-        <v>-0.004109892144370811</v>
-      </c>
-      <c r="E641" t="n">
-        <v>-0.002220440031184795</v>
-      </c>
-      <c r="F641" t="n">
-        <v>0.00205243428460597</v>
-      </c>
-      <c r="G641" t="n">
-        <v>0.004053646541112538</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>